<commit_message>
update Inputs12 (re-add code for source)
</commit_message>
<xml_diff>
--- a/inputs/Inputs12.xlsx
+++ b/inputs/Inputs12.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="741" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SETTING" sheetId="6" r:id="rId1"/>
@@ -396,8 +396,8 @@
     <author>tc={B7E55C45-E04A-4F94-86D3-DB2FF5464B13}</author>
     <author>tc={CC05E439-91CA-4296-9258-92175AA92058}</author>
     <author>tc={95B0448B-4542-45B3-9B74-3DA0C9AF60E7}</author>
+    <author>PhuongPQ</author>
     <author>tc={358A766E-B6D1-4484-A68D-C6AF472CBC6E}</author>
-    <author>PhuongPQ</author>
     <author>tc={57748AED-F455-477B-A70E-41AA9060EA7C}</author>
   </authors>
   <commentList>
@@ -461,6 +461,21 @@
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>0: feeder or Swing BUS
+1: Generator of PV BUS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="5" shapeId="0">
+      <text>
+        <r>
+          <rPr>
             <sz val="11"/>
             <color theme="1"/>
             <rFont val="Calibri"/>
@@ -471,7 +486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="4" shapeId="0">
+    <comment ref="H2" authorId="5" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -485,7 +500,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="5" shapeId="0">
+    <comment ref="I2" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -509,7 +524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="6" shapeId="0">
+    <comment ref="J2" authorId="6" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -524,7 +539,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="6" shapeId="0">
+    <comment ref="K2" authorId="6" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -539,7 +554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="5" shapeId="0">
+    <comment ref="L2" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -553,7 +568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="5" shapeId="0">
+    <comment ref="M2" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -567,7 +582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="5" shapeId="0">
+    <comment ref="N2" authorId="4" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1551,7 +1566,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="103">
   <si>
     <t>NAME</t>
   </si>
@@ -1838,9 +1853,6 @@
     <t>i0     [%]</t>
   </si>
   <si>
-    <t>dP   [kw]</t>
-  </si>
-  <si>
     <t>NAME1</t>
   </si>
   <si>
@@ -1857,6 +1869,12 @@
   </si>
   <si>
     <t>deltaP   [kW]</t>
+  </si>
+  <si>
+    <t>CODE</t>
+  </si>
+  <si>
+    <t>deltaP   [kw]</t>
   </si>
 </sst>
 </file>
@@ -2070,13 +2088,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>43484</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>422413</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>542848</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>177114</xdr:rowOff>
@@ -2156,16 +2174,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>358221</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>310596</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>143289</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>487039</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>49624</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>217641</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>182973</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2182,8 +2200,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13159821" y="981489"/>
-          <a:ext cx="4396018" cy="4068760"/>
+          <a:off x="1644096" y="914400"/>
+          <a:ext cx="3202695" cy="2964273"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2206,7 +2224,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>391375</xdr:colOff>
+      <xdr:colOff>391376</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>121684</xdr:rowOff>
     </xdr:to>
@@ -2646,7 +2664,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2802,8 +2820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2812,9 +2830,10 @@
     <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" style="1" customWidth="1"/>
     <col min="4" max="5" width="8.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="8" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3276,11 +3295,19 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="max"/>
         <color rgb="FFFF7128"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="5"/>
         <color theme="0"/>
       </colorScale>
     </cfRule>
@@ -3294,10 +3321,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3307,24 +3334,25 @@
     <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="7.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="7.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H1"/>
       <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
-    </row>
-    <row r="2" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L1"/>
+    </row>
+    <row r="2" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>65</v>
       </c>
@@ -3340,32 +3368,35 @@
       <c r="E2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3381,24 +3412,27 @@
       <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
         <v>1.02</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>15</v>
       </c>
-      <c r="I3" s="1">
-        <v>9999</v>
-      </c>
       <c r="J3" s="1">
-        <v>-9999</v>
+        <v>99999</v>
       </c>
       <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-99999</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3412,31 +3446,54 @@
         <v>12</v>
       </c>
       <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
         <v>1.02</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>15</v>
       </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
       <c r="I4" s="1">
-        <v>9999</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>-9999</v>
+        <v>99999</v>
       </c>
       <c r="K4" s="1">
-        <v>0</v>
+        <v>-99999</v>
       </c>
       <c r="L4" s="1">
         <v>0</v>
       </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color rgb="FFFFFF00"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFFFF00"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -3449,7 +3506,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3485,7 +3542,7 @@
         <v>49</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>14</v>
@@ -3573,6 +3630,16 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFFFF00"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -3588,7 +3655,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3634,10 +3701,10 @@
         <v>82</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>31</v>
@@ -4208,7 +4275,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="1">
         <v>1</v>
@@ -4329,6 +4396,47 @@
       </c>
       <c r="Q17" s="1">
         <v>-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>10</v>
+      </c>
+      <c r="C18" s="1">
+        <v>11</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -4360,7 +4468,7 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4368,7 +4476,8 @@
     <col min="1" max="1" width="7.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="14.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="4" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -4403,16 +4512,16 @@
         <v>82</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>31</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>14</v>
@@ -4656,6 +4765,16 @@
       <c r="O25" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF7128"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -4667,8 +4786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4676,9 +4795,9 @@
     <col min="1" max="1" width="7.140625" style="1" customWidth="1"/>
     <col min="2" max="3" width="8.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -4730,19 +4849,19 @@
         <v>83</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>31</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J2" s="11" t="s">
         <v>14</v>
@@ -5104,6 +5223,16 @@
       <c r="W25" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF7128"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -5116,7 +5245,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5426,7 +5555,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G4"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5457,7 +5586,7 @@
         <v>74</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>14</v>
@@ -5507,6 +5636,16 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF7128"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>